<commit_message>
Written detailed planning and introduction in documentation.
</commit_message>
<xml_diff>
--- a/2_Documentation/2_Project_Planning/GANTT.xlsx
+++ b/2_Documentation/2_Project_Planning/GANTT.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="189" documentId="13_ncr:1_{B83F1FDC-9097-4D23-B056-F10483920BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1FEED3FB-157E-4697-89B7-DCAD25CBD7FE}"/>
+  <xr:revisionPtr revIDLastSave="196" documentId="13_ncr:1_{B83F1FDC-9097-4D23-B056-F10483920BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCC8FE5B-143B-4A42-847E-9F5E1A1581BB}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -586,7 +586,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -650,6 +650,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="8" xfId="6" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="11" xfId="6" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -674,44 +707,8 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="9" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="8" xfId="6" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="11" xfId="6" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -889,6 +886,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1125,7 +1126,7 @@
   <dimension ref="B1:AL24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1154,10 +1155,10 @@
       </c>
       <c r="D2" s="17"/>
       <c r="E2" s="11"/>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="22"/>
+      <c r="G2" s="33"/>
       <c r="H2" s="12"/>
       <c r="I2" s="18" t="s">
         <v>1</v>
@@ -1165,43 +1166,43 @@
       <c r="J2" s="19"/>
       <c r="K2" s="19"/>
       <c r="L2" s="13"/>
-      <c r="M2" s="23" t="s">
+      <c r="M2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
       <c r="R2" s="14"/>
-      <c r="S2" s="23" t="s">
+      <c r="S2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="T2" s="24"/>
-      <c r="U2" s="24"/>
-      <c r="V2" s="24"/>
-      <c r="W2" s="24"/>
-      <c r="X2" s="24"/>
-      <c r="Y2" s="24"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="35"/>
+      <c r="V2" s="35"/>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="35"/>
       <c r="Z2" s="19"/>
       <c r="AA2" s="19"/>
     </row>
     <row r="3" spans="2:38" s="7" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="25" t="s">
+      <c r="B3" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="36" t="s">
         <v>8</v>
       </c>
       <c r="H3" s="15" t="s">
@@ -1211,11 +1212,10 @@
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
-      <c r="M3" s="35" t="s">
+      <c r="N3" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="N3" s="35"/>
-      <c r="O3" s="36"/>
+      <c r="O3" s="40"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
       <c r="R3" s="6"/>
@@ -1225,15 +1225,15 @@
       <c r="V3" s="6"/>
       <c r="W3" s="6"/>
       <c r="X3" s="6"/>
-      <c r="Y3" s="34"/>
+      <c r="Y3" s="26"/>
     </row>
     <row r="4" spans="2:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="28"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
       <c r="H4" s="3">
         <v>35</v>
       </c>
@@ -1307,753 +1307,753 @@
       </c>
     </row>
     <row r="5" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="22">
         <v>36</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="22">
         <v>3</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="22">
         <v>36</v>
       </c>
-      <c r="F5" s="30">
+      <c r="F5" s="22">
         <v>4</v>
       </c>
-      <c r="G5" s="33">
+      <c r="G5" s="25">
         <v>0.8</v>
       </c>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31"/>
-      <c r="Q5" s="31"/>
-      <c r="R5" s="31"/>
-      <c r="S5" s="31"/>
-      <c r="T5" s="31"/>
-      <c r="U5" s="31"/>
-      <c r="V5" s="31"/>
-      <c r="W5" s="31"/>
-      <c r="X5" s="31"/>
-      <c r="Y5" s="32"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="23"/>
+      <c r="V5" s="23"/>
+      <c r="W5" s="23"/>
+      <c r="X5" s="23"/>
+      <c r="Y5" s="24"/>
     </row>
     <row r="6" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="22">
         <v>39</v>
       </c>
-      <c r="D6" s="30">
+      <c r="D6" s="22">
         <v>1</v>
       </c>
-      <c r="E6" s="30">
-        <v>0</v>
-      </c>
-      <c r="F6" s="30">
-        <v>0</v>
-      </c>
-      <c r="G6" s="33">
-        <v>0</v>
-      </c>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="31"/>
-      <c r="N6" s="31"/>
-      <c r="O6" s="31"/>
-      <c r="P6" s="31"/>
-      <c r="Q6" s="31"/>
-      <c r="R6" s="31"/>
-      <c r="S6" s="31"/>
-      <c r="T6" s="31"/>
-      <c r="U6" s="31"/>
-      <c r="V6" s="31"/>
-      <c r="W6" s="31"/>
-      <c r="X6" s="31"/>
-      <c r="Y6" s="32"/>
+      <c r="E6" s="22">
+        <v>0</v>
+      </c>
+      <c r="F6" s="22">
+        <v>0</v>
+      </c>
+      <c r="G6" s="25">
+        <v>0</v>
+      </c>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="23"/>
+      <c r="T6" s="23"/>
+      <c r="U6" s="23"/>
+      <c r="V6" s="23"/>
+      <c r="W6" s="23"/>
+      <c r="X6" s="23"/>
+      <c r="Y6" s="24"/>
     </row>
     <row r="7" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="22">
         <v>39</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="22">
         <v>2</v>
       </c>
-      <c r="E7" s="30">
-        <v>0</v>
-      </c>
-      <c r="F7" s="30">
-        <v>0</v>
-      </c>
-      <c r="G7" s="33">
-        <v>0</v>
-      </c>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="31"/>
-      <c r="O7" s="31"/>
-      <c r="P7" s="31"/>
-      <c r="Q7" s="31"/>
-      <c r="R7" s="31"/>
-      <c r="S7" s="31"/>
-      <c r="T7" s="31"/>
-      <c r="U7" s="31"/>
-      <c r="V7" s="31"/>
-      <c r="W7" s="31"/>
-      <c r="X7" s="31"/>
-      <c r="Y7" s="32"/>
+      <c r="E7" s="22">
+        <v>0</v>
+      </c>
+      <c r="F7" s="22">
+        <v>0</v>
+      </c>
+      <c r="G7" s="25">
+        <v>0</v>
+      </c>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="23"/>
+      <c r="U7" s="23"/>
+      <c r="V7" s="23"/>
+      <c r="W7" s="23"/>
+      <c r="X7" s="23"/>
+      <c r="Y7" s="24"/>
     </row>
     <row r="8" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="30">
+      <c r="C8" s="22">
         <v>40</v>
       </c>
-      <c r="D8" s="30">
+      <c r="D8" s="22">
         <v>2</v>
       </c>
-      <c r="E8" s="30">
-        <v>0</v>
-      </c>
-      <c r="F8" s="30">
-        <v>0</v>
-      </c>
-      <c r="G8" s="33">
-        <v>0</v>
-      </c>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31"/>
-      <c r="Q8" s="31"/>
-      <c r="R8" s="31"/>
-      <c r="S8" s="31"/>
-      <c r="T8" s="31"/>
-      <c r="U8" s="31"/>
-      <c r="V8" s="31"/>
-      <c r="W8" s="31"/>
-      <c r="X8" s="31"/>
-      <c r="Y8" s="32"/>
+      <c r="E8" s="22">
+        <v>0</v>
+      </c>
+      <c r="F8" s="22">
+        <v>0</v>
+      </c>
+      <c r="G8" s="25">
+        <v>0</v>
+      </c>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="23"/>
+      <c r="S8" s="23"/>
+      <c r="T8" s="23"/>
+      <c r="U8" s="23"/>
+      <c r="V8" s="23"/>
+      <c r="W8" s="23"/>
+      <c r="X8" s="23"/>
+      <c r="Y8" s="24"/>
       <c r="AL8" s="20"/>
     </row>
     <row r="9" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="30">
+      <c r="C9" s="22">
         <v>43</v>
       </c>
-      <c r="D9" s="30">
+      <c r="D9" s="22">
         <v>1</v>
       </c>
-      <c r="E9" s="30">
-        <v>0</v>
-      </c>
-      <c r="F9" s="30">
-        <v>0</v>
-      </c>
-      <c r="G9" s="33">
-        <v>0</v>
-      </c>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="31"/>
-      <c r="N9" s="31"/>
-      <c r="O9" s="31"/>
-      <c r="P9" s="31"/>
-      <c r="Q9" s="31"/>
-      <c r="R9" s="31"/>
-      <c r="S9" s="31"/>
-      <c r="T9" s="31"/>
-      <c r="U9" s="31"/>
-      <c r="V9" s="31"/>
-      <c r="W9" s="31"/>
-      <c r="X9" s="31"/>
-      <c r="Y9" s="32"/>
+      <c r="E9" s="22">
+        <v>0</v>
+      </c>
+      <c r="F9" s="22">
+        <v>0</v>
+      </c>
+      <c r="G9" s="25">
+        <v>0</v>
+      </c>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="23"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="23"/>
+      <c r="T9" s="23"/>
+      <c r="U9" s="23"/>
+      <c r="V9" s="23"/>
+      <c r="W9" s="23"/>
+      <c r="X9" s="23"/>
+      <c r="Y9" s="24"/>
     </row>
     <row r="10" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="30">
-        <v>40</v>
-      </c>
-      <c r="D10" s="30">
+      <c r="C10" s="22">
+        <v>41</v>
+      </c>
+      <c r="D10" s="22">
         <v>2</v>
       </c>
-      <c r="E10" s="30">
-        <v>0</v>
-      </c>
-      <c r="F10" s="30">
-        <v>0</v>
-      </c>
-      <c r="G10" s="33">
-        <v>0</v>
-      </c>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="31"/>
-      <c r="O10" s="31"/>
-      <c r="P10" s="31"/>
-      <c r="Q10" s="31"/>
-      <c r="R10" s="31"/>
-      <c r="S10" s="31"/>
-      <c r="T10" s="31"/>
-      <c r="U10" s="31"/>
-      <c r="V10" s="31"/>
-      <c r="W10" s="31"/>
-      <c r="X10" s="31"/>
-      <c r="Y10" s="32"/>
+      <c r="E10" s="22">
+        <v>0</v>
+      </c>
+      <c r="F10" s="22">
+        <v>0</v>
+      </c>
+      <c r="G10" s="25">
+        <v>0</v>
+      </c>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
+      <c r="Q10" s="23"/>
+      <c r="R10" s="23"/>
+      <c r="S10" s="23"/>
+      <c r="T10" s="23"/>
+      <c r="U10" s="23"/>
+      <c r="V10" s="23"/>
+      <c r="W10" s="23"/>
+      <c r="X10" s="23"/>
+      <c r="Y10" s="24"/>
     </row>
     <row r="11" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="30">
+      <c r="C11" s="22">
         <v>42</v>
       </c>
-      <c r="D11" s="30">
+      <c r="D11" s="22">
         <v>2</v>
       </c>
-      <c r="E11" s="30">
-        <v>0</v>
-      </c>
-      <c r="F11" s="30">
-        <v>0</v>
-      </c>
-      <c r="G11" s="33">
-        <v>0</v>
-      </c>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="31"/>
-      <c r="P11" s="31"/>
-      <c r="Q11" s="31"/>
-      <c r="R11" s="31"/>
-      <c r="S11" s="31"/>
-      <c r="T11" s="31"/>
-      <c r="U11" s="31"/>
-      <c r="V11" s="31"/>
-      <c r="W11" s="31"/>
-      <c r="X11" s="31"/>
-      <c r="Y11" s="32"/>
+      <c r="E11" s="22">
+        <v>0</v>
+      </c>
+      <c r="F11" s="22">
+        <v>0</v>
+      </c>
+      <c r="G11" s="25">
+        <v>0</v>
+      </c>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="23"/>
+      <c r="S11" s="23"/>
+      <c r="T11" s="23"/>
+      <c r="U11" s="23"/>
+      <c r="V11" s="23"/>
+      <c r="W11" s="23"/>
+      <c r="X11" s="23"/>
+      <c r="Y11" s="24"/>
     </row>
     <row r="12" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="30">
+      <c r="C12" s="22">
         <v>42</v>
       </c>
-      <c r="D12" s="30">
+      <c r="D12" s="22">
         <v>2</v>
       </c>
-      <c r="E12" s="30">
-        <v>0</v>
-      </c>
-      <c r="F12" s="30">
-        <v>0</v>
-      </c>
-      <c r="G12" s="33">
-        <v>0</v>
-      </c>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="31"/>
-      <c r="O12" s="31"/>
-      <c r="P12" s="31"/>
-      <c r="Q12" s="31"/>
-      <c r="R12" s="31"/>
-      <c r="S12" s="31"/>
-      <c r="T12" s="31"/>
-      <c r="U12" s="31"/>
-      <c r="V12" s="31"/>
-      <c r="W12" s="31"/>
-      <c r="X12" s="31"/>
-      <c r="Y12" s="32"/>
+      <c r="E12" s="22">
+        <v>0</v>
+      </c>
+      <c r="F12" s="22">
+        <v>0</v>
+      </c>
+      <c r="G12" s="25">
+        <v>0</v>
+      </c>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="23"/>
+      <c r="R12" s="23"/>
+      <c r="S12" s="23"/>
+      <c r="T12" s="23"/>
+      <c r="U12" s="23"/>
+      <c r="V12" s="23"/>
+      <c r="W12" s="23"/>
+      <c r="X12" s="23"/>
+      <c r="Y12" s="24"/>
     </row>
     <row r="13" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="30">
+      <c r="C13" s="22">
         <v>44</v>
       </c>
-      <c r="D13" s="30">
+      <c r="D13" s="22">
         <v>1</v>
       </c>
-      <c r="E13" s="30">
-        <v>0</v>
-      </c>
-      <c r="F13" s="30">
-        <v>0</v>
-      </c>
-      <c r="G13" s="33">
-        <v>0</v>
-      </c>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="31"/>
-      <c r="M13" s="31"/>
-      <c r="N13" s="31"/>
-      <c r="O13" s="31"/>
-      <c r="P13" s="31"/>
-      <c r="Q13" s="31"/>
-      <c r="R13" s="31"/>
-      <c r="S13" s="31"/>
-      <c r="T13" s="31"/>
-      <c r="U13" s="31"/>
-      <c r="V13" s="31"/>
-      <c r="W13" s="31"/>
-      <c r="X13" s="31"/>
-      <c r="Y13" s="32"/>
+      <c r="E13" s="22">
+        <v>0</v>
+      </c>
+      <c r="F13" s="22">
+        <v>0</v>
+      </c>
+      <c r="G13" s="25">
+        <v>0</v>
+      </c>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="23"/>
+      <c r="R13" s="23"/>
+      <c r="S13" s="23"/>
+      <c r="T13" s="23"/>
+      <c r="U13" s="23"/>
+      <c r="V13" s="23"/>
+      <c r="W13" s="23"/>
+      <c r="X13" s="23"/>
+      <c r="Y13" s="24"/>
     </row>
     <row r="14" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="30">
+      <c r="C14" s="22">
         <v>45</v>
       </c>
-      <c r="D14" s="30">
+      <c r="D14" s="22">
         <v>1</v>
       </c>
-      <c r="E14" s="30">
-        <v>0</v>
-      </c>
-      <c r="F14" s="30">
-        <v>0</v>
-      </c>
-      <c r="G14" s="33">
-        <v>0</v>
-      </c>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="31"/>
-      <c r="M14" s="31"/>
-      <c r="N14" s="31"/>
-      <c r="O14" s="31"/>
-      <c r="P14" s="31"/>
-      <c r="Q14" s="31"/>
-      <c r="R14" s="31"/>
-      <c r="S14" s="31"/>
-      <c r="T14" s="31"/>
-      <c r="U14" s="31"/>
-      <c r="V14" s="31"/>
-      <c r="W14" s="31"/>
-      <c r="X14" s="31"/>
-      <c r="Y14" s="32"/>
+      <c r="E14" s="22">
+        <v>0</v>
+      </c>
+      <c r="F14" s="22">
+        <v>0</v>
+      </c>
+      <c r="G14" s="25">
+        <v>0</v>
+      </c>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="23"/>
+      <c r="R14" s="23"/>
+      <c r="S14" s="23"/>
+      <c r="T14" s="23"/>
+      <c r="U14" s="23"/>
+      <c r="V14" s="23"/>
+      <c r="W14" s="23"/>
+      <c r="X14" s="23"/>
+      <c r="Y14" s="24"/>
     </row>
     <row r="15" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="30">
+      <c r="C15" s="22">
         <v>46</v>
       </c>
-      <c r="D15" s="30">
+      <c r="D15" s="22">
         <v>3</v>
       </c>
-      <c r="E15" s="30">
-        <v>0</v>
-      </c>
-      <c r="F15" s="30">
-        <v>0</v>
-      </c>
-      <c r="G15" s="33">
-        <v>0</v>
-      </c>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="31"/>
-      <c r="L15" s="31"/>
-      <c r="M15" s="31"/>
-      <c r="N15" s="31"/>
-      <c r="O15" s="31"/>
-      <c r="P15" s="31"/>
-      <c r="Q15" s="31"/>
-      <c r="R15" s="31"/>
-      <c r="S15" s="31"/>
-      <c r="T15" s="31"/>
-      <c r="U15" s="31"/>
-      <c r="V15" s="31"/>
-      <c r="W15" s="31"/>
-      <c r="X15" s="31"/>
-      <c r="Y15" s="32"/>
+      <c r="E15" s="22">
+        <v>0</v>
+      </c>
+      <c r="F15" s="22">
+        <v>0</v>
+      </c>
+      <c r="G15" s="25">
+        <v>0</v>
+      </c>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="23"/>
+      <c r="R15" s="23"/>
+      <c r="S15" s="23"/>
+      <c r="T15" s="23"/>
+      <c r="U15" s="23"/>
+      <c r="V15" s="23"/>
+      <c r="W15" s="23"/>
+      <c r="X15" s="23"/>
+      <c r="Y15" s="24"/>
     </row>
     <row r="16" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="30">
+      <c r="C16" s="22">
         <v>49</v>
       </c>
-      <c r="D16" s="30">
+      <c r="D16" s="22">
         <v>3</v>
       </c>
-      <c r="E16" s="30">
-        <v>0</v>
-      </c>
-      <c r="F16" s="30">
-        <v>0</v>
-      </c>
-      <c r="G16" s="33">
-        <v>0</v>
-      </c>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
-      <c r="K16" s="31"/>
-      <c r="L16" s="31"/>
-      <c r="M16" s="31"/>
-      <c r="N16" s="31"/>
-      <c r="O16" s="31"/>
-      <c r="P16" s="31"/>
-      <c r="Q16" s="31"/>
-      <c r="R16" s="31"/>
-      <c r="S16" s="31"/>
-      <c r="T16" s="31"/>
-      <c r="U16" s="31"/>
-      <c r="V16" s="31"/>
-      <c r="W16" s="31"/>
-      <c r="X16" s="31"/>
-      <c r="Y16" s="32"/>
+      <c r="E16" s="22">
+        <v>0</v>
+      </c>
+      <c r="F16" s="22">
+        <v>0</v>
+      </c>
+      <c r="G16" s="25">
+        <v>0</v>
+      </c>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="23"/>
+      <c r="R16" s="23"/>
+      <c r="S16" s="23"/>
+      <c r="T16" s="23"/>
+      <c r="U16" s="23"/>
+      <c r="V16" s="23"/>
+      <c r="W16" s="23"/>
+      <c r="X16" s="23"/>
+      <c r="Y16" s="24"/>
     </row>
     <row r="17" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="30">
+      <c r="C17" s="22">
         <v>49</v>
       </c>
-      <c r="D17" s="30">
+      <c r="D17" s="22">
         <v>3</v>
       </c>
-      <c r="E17" s="30">
-        <v>0</v>
-      </c>
-      <c r="F17" s="30">
-        <v>0</v>
-      </c>
-      <c r="G17" s="33">
-        <v>0</v>
-      </c>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="31"/>
-      <c r="L17" s="31"/>
-      <c r="M17" s="31"/>
-      <c r="N17" s="31"/>
-      <c r="O17" s="31"/>
-      <c r="P17" s="31"/>
-      <c r="Q17" s="31"/>
-      <c r="R17" s="31"/>
-      <c r="S17" s="31"/>
-      <c r="T17" s="31"/>
-      <c r="U17" s="31"/>
-      <c r="V17" s="31"/>
-      <c r="W17" s="31"/>
-      <c r="X17" s="31"/>
-      <c r="Y17" s="32"/>
+      <c r="E17" s="22">
+        <v>0</v>
+      </c>
+      <c r="F17" s="22">
+        <v>0</v>
+      </c>
+      <c r="G17" s="25">
+        <v>0</v>
+      </c>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="23"/>
+      <c r="R17" s="23"/>
+      <c r="S17" s="23"/>
+      <c r="T17" s="23"/>
+      <c r="U17" s="23"/>
+      <c r="V17" s="23"/>
+      <c r="W17" s="23"/>
+      <c r="X17" s="23"/>
+      <c r="Y17" s="24"/>
     </row>
     <row r="18" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="30">
+      <c r="C18" s="22">
         <v>51</v>
       </c>
-      <c r="D18" s="30">
+      <c r="D18" s="22">
         <v>1</v>
       </c>
-      <c r="E18" s="30">
-        <v>0</v>
-      </c>
-      <c r="F18" s="30">
-        <v>0</v>
-      </c>
-      <c r="G18" s="33">
-        <v>0</v>
-      </c>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="31"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="31"/>
-      <c r="N18" s="31"/>
-      <c r="O18" s="31"/>
-      <c r="P18" s="31"/>
-      <c r="Q18" s="31"/>
-      <c r="R18" s="31"/>
-      <c r="S18" s="31"/>
-      <c r="T18" s="31"/>
-      <c r="U18" s="31"/>
-      <c r="V18" s="31"/>
-      <c r="W18" s="31"/>
-      <c r="X18" s="31"/>
-      <c r="Y18" s="32"/>
+      <c r="E18" s="22">
+        <v>0</v>
+      </c>
+      <c r="F18" s="22">
+        <v>0</v>
+      </c>
+      <c r="G18" s="25">
+        <v>0</v>
+      </c>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="23"/>
+      <c r="P18" s="23"/>
+      <c r="Q18" s="23"/>
+      <c r="R18" s="23"/>
+      <c r="S18" s="23"/>
+      <c r="T18" s="23"/>
+      <c r="U18" s="23"/>
+      <c r="V18" s="23"/>
+      <c r="W18" s="23"/>
+      <c r="X18" s="23"/>
+      <c r="Y18" s="24"/>
     </row>
     <row r="19" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="29"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="31"/>
-      <c r="L19" s="31"/>
-      <c r="M19" s="31"/>
-      <c r="N19" s="31"/>
-      <c r="O19" s="31"/>
-      <c r="P19" s="31"/>
-      <c r="Q19" s="31"/>
-      <c r="R19" s="31"/>
-      <c r="S19" s="31"/>
-      <c r="T19" s="31"/>
-      <c r="U19" s="31"/>
-      <c r="V19" s="31"/>
-      <c r="W19" s="31"/>
-      <c r="X19" s="31"/>
-      <c r="Y19" s="32"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="23"/>
+      <c r="R19" s="23"/>
+      <c r="S19" s="23"/>
+      <c r="T19" s="23"/>
+      <c r="U19" s="23"/>
+      <c r="V19" s="23"/>
+      <c r="W19" s="23"/>
+      <c r="X19" s="23"/>
+      <c r="Y19" s="24"/>
     </row>
     <row r="20" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="30">
+      <c r="C20" s="22">
         <v>38</v>
       </c>
-      <c r="D20" s="30">
+      <c r="D20" s="22">
         <v>14</v>
       </c>
-      <c r="E20" s="30">
-        <v>0</v>
-      </c>
-      <c r="F20" s="30">
-        <v>0</v>
-      </c>
-      <c r="G20" s="33">
-        <v>0</v>
-      </c>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="31"/>
-      <c r="L20" s="31"/>
-      <c r="M20" s="31"/>
-      <c r="N20" s="31"/>
-      <c r="O20" s="31"/>
-      <c r="P20" s="31"/>
-      <c r="Q20" s="31"/>
-      <c r="R20" s="31"/>
-      <c r="S20" s="31"/>
-      <c r="T20" s="31"/>
-      <c r="U20" s="31"/>
-      <c r="V20" s="31"/>
-      <c r="W20" s="31"/>
-      <c r="X20" s="31"/>
-      <c r="Y20" s="32"/>
+      <c r="E20" s="22">
+        <v>0</v>
+      </c>
+      <c r="F20" s="22">
+        <v>0</v>
+      </c>
+      <c r="G20" s="25">
+        <v>0</v>
+      </c>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="23"/>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="23"/>
+      <c r="R20" s="23"/>
+      <c r="S20" s="23"/>
+      <c r="T20" s="23"/>
+      <c r="U20" s="23"/>
+      <c r="V20" s="23"/>
+      <c r="W20" s="23"/>
+      <c r="X20" s="23"/>
+      <c r="Y20" s="24"/>
     </row>
     <row r="21" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="30">
+      <c r="C21" s="22">
         <v>38</v>
       </c>
-      <c r="D21" s="30">
+      <c r="D21" s="22">
         <v>14</v>
       </c>
-      <c r="E21" s="30">
-        <v>0</v>
-      </c>
-      <c r="F21" s="30">
-        <v>0</v>
-      </c>
-      <c r="G21" s="33">
-        <v>0</v>
-      </c>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="31"/>
-      <c r="L21" s="31"/>
-      <c r="M21" s="31"/>
-      <c r="N21" s="31"/>
-      <c r="O21" s="31"/>
-      <c r="P21" s="31"/>
-      <c r="Q21" s="31"/>
-      <c r="R21" s="31"/>
-      <c r="S21" s="31"/>
-      <c r="T21" s="31"/>
-      <c r="U21" s="31"/>
-      <c r="V21" s="31"/>
-      <c r="W21" s="31"/>
-      <c r="X21" s="31"/>
-      <c r="Y21" s="32"/>
+      <c r="E21" s="22">
+        <v>0</v>
+      </c>
+      <c r="F21" s="22">
+        <v>0</v>
+      </c>
+      <c r="G21" s="25">
+        <v>0</v>
+      </c>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="23"/>
+      <c r="O21" s="23"/>
+      <c r="P21" s="23"/>
+      <c r="Q21" s="23"/>
+      <c r="R21" s="23"/>
+      <c r="S21" s="23"/>
+      <c r="T21" s="23"/>
+      <c r="U21" s="23"/>
+      <c r="V21" s="23"/>
+      <c r="W21" s="23"/>
+      <c r="X21" s="23"/>
+      <c r="Y21" s="24"/>
     </row>
     <row r="22" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="30">
+      <c r="C22" s="22">
         <v>38</v>
       </c>
-      <c r="D22" s="30">
+      <c r="D22" s="22">
         <v>14</v>
       </c>
-      <c r="E22" s="30">
-        <v>0</v>
-      </c>
-      <c r="F22" s="30">
-        <v>0</v>
-      </c>
-      <c r="G22" s="33">
-        <v>0</v>
-      </c>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31"/>
-      <c r="L22" s="31"/>
-      <c r="M22" s="31"/>
-      <c r="N22" s="31"/>
-      <c r="O22" s="31"/>
-      <c r="P22" s="31"/>
-      <c r="Q22" s="31"/>
-      <c r="R22" s="31"/>
-      <c r="S22" s="31"/>
-      <c r="T22" s="31"/>
-      <c r="U22" s="31"/>
-      <c r="V22" s="31"/>
-      <c r="W22" s="31"/>
-      <c r="X22" s="31"/>
-      <c r="Y22" s="32"/>
+      <c r="E22" s="22">
+        <v>0</v>
+      </c>
+      <c r="F22" s="22">
+        <v>0</v>
+      </c>
+      <c r="G22" s="25">
+        <v>0</v>
+      </c>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="23"/>
+      <c r="O22" s="23"/>
+      <c r="P22" s="23"/>
+      <c r="Q22" s="23"/>
+      <c r="R22" s="23"/>
+      <c r="S22" s="23"/>
+      <c r="T22" s="23"/>
+      <c r="U22" s="23"/>
+      <c r="V22" s="23"/>
+      <c r="W22" s="23"/>
+      <c r="X22" s="23"/>
+      <c r="Y22" s="24"/>
     </row>
     <row r="23" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="30">
+      <c r="C23" s="22">
         <v>43</v>
       </c>
-      <c r="D23" s="30">
+      <c r="D23" s="22">
         <v>1</v>
       </c>
-      <c r="E23" s="30">
-        <v>0</v>
-      </c>
-      <c r="F23" s="30">
-        <v>0</v>
-      </c>
-      <c r="G23" s="33">
-        <v>0</v>
-      </c>
-      <c r="H23" s="31"/>
-      <c r="I23" s="31"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="31"/>
-      <c r="L23" s="31"/>
-      <c r="M23" s="31"/>
-      <c r="N23" s="31"/>
-      <c r="O23" s="31"/>
-      <c r="P23" s="31"/>
-      <c r="Q23" s="31"/>
-      <c r="R23" s="31"/>
-      <c r="S23" s="31"/>
-      <c r="T23" s="31"/>
-      <c r="U23" s="31"/>
-      <c r="V23" s="31"/>
-      <c r="W23" s="31"/>
-      <c r="X23" s="31"/>
-      <c r="Y23" s="32"/>
+      <c r="E23" s="22">
+        <v>0</v>
+      </c>
+      <c r="F23" s="22">
+        <v>0</v>
+      </c>
+      <c r="G23" s="25">
+        <v>0</v>
+      </c>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="23"/>
+      <c r="O23" s="23"/>
+      <c r="P23" s="23"/>
+      <c r="Q23" s="23"/>
+      <c r="R23" s="23"/>
+      <c r="S23" s="23"/>
+      <c r="T23" s="23"/>
+      <c r="U23" s="23"/>
+      <c r="V23" s="23"/>
+      <c r="W23" s="23"/>
+      <c r="X23" s="23"/>
+      <c r="Y23" s="24"/>
     </row>
     <row r="24" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="37" t="s">
+      <c r="B24" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="38">
+      <c r="C24" s="28">
         <v>48</v>
       </c>
-      <c r="D24" s="38">
+      <c r="D24" s="28">
         <v>1</v>
       </c>
-      <c r="E24" s="38">
-        <v>0</v>
-      </c>
-      <c r="F24" s="38">
-        <v>0</v>
-      </c>
-      <c r="G24" s="39">
-        <v>0</v>
-      </c>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
-      <c r="M24" s="40"/>
-      <c r="N24" s="40"/>
-      <c r="O24" s="40"/>
-      <c r="P24" s="40"/>
-      <c r="Q24" s="40"/>
-      <c r="R24" s="40"/>
-      <c r="S24" s="40"/>
-      <c r="T24" s="40"/>
-      <c r="U24" s="40"/>
-      <c r="V24" s="40"/>
-      <c r="W24" s="40"/>
-      <c r="X24" s="40"/>
-      <c r="Y24" s="41"/>
+      <c r="E24" s="28">
+        <v>0</v>
+      </c>
+      <c r="F24" s="28">
+        <v>0</v>
+      </c>
+      <c r="G24" s="29">
+        <v>0</v>
+      </c>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="30"/>
+      <c r="L24" s="30"/>
+      <c r="M24" s="30"/>
+      <c r="N24" s="30"/>
+      <c r="O24" s="30"/>
+      <c r="P24" s="30"/>
+      <c r="Q24" s="30"/>
+      <c r="R24" s="30"/>
+      <c r="S24" s="30"/>
+      <c r="T24" s="30"/>
+      <c r="U24" s="30"/>
+      <c r="V24" s="30"/>
+      <c r="W24" s="30"/>
+      <c r="X24" s="30"/>
+      <c r="Y24" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -2066,7 +2066,7 @@
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="N3:O3"/>
   </mergeCells>
   <conditionalFormatting sqref="B25:Y25">
     <cfRule type="expression" dxfId="9" priority="2">

</xml_diff>

<commit_message>
Documentation: Journal and GANTT updates.
</commit_message>
<xml_diff>
--- a/2_Documentation/2_Project_Planning/GANTT.xlsx
+++ b/2_Documentation/2_Project_Planning/GANTT.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20403"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="214" documentId="13_ncr:1_{B83F1FDC-9097-4D23-B056-F10483920BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2354FD38-5B1F-4F74-BB5E-24291FF82C6E}"/>
+  <xr:revisionPtr revIDLastSave="228" documentId="13_ncr:1_{B83F1FDC-9097-4D23-B056-F10483920BA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{D09831FD-2CC5-4D23-9274-4EA28E674E67}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="28995" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -13,27 +13,17 @@
   <definedNames>
     <definedName name="Actual">(PeriodInActual*('Project Planner'!$E1&gt;0))*PeriodInPlan</definedName>
     <definedName name="ActualBeyond">PeriodInActual*('Project Planner'!$E1&gt;0)</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Project Planner'!$3:$4</definedName>
     <definedName name="PercentComplete">PercentCompleteBeyond*PeriodInPlan</definedName>
     <definedName name="PercentCompleteBeyond">('Project Planner'!A$4=MEDIAN('Project Planner'!A$4,'Project Planner'!$E1,'Project Planner'!$E1+'Project Planner'!$F1)*('Project Planner'!$E1&gt;0))*(('Project Planner'!A$4&lt;(INT('Project Planner'!$E1+'Project Planner'!$F1*'Project Planner'!$G1)))+('Project Planner'!A$4='Project Planner'!$E1))*('Project Planner'!$G1&gt;0)</definedName>
     <definedName name="period_selected">'Project Planner'!#REF!</definedName>
     <definedName name="PeriodInActual">'Project Planner'!A$4=MEDIAN('Project Planner'!A$4,'Project Planner'!$E1,'Project Planner'!$E1+'Project Planner'!$F1-1)</definedName>
     <definedName name="PeriodInPlan">'Project Planner'!A$4=MEDIAN('Project Planner'!A$4,'Project Planner'!$C1,'Project Planner'!$C1+'Project Planner'!$D1-1)</definedName>
     <definedName name="Plan">PeriodInPlan*('Project Planner'!$C1&gt;0)</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Project Planner'!$3:$4</definedName>
     <definedName name="TitleRegion..BO60">'Project Planner'!$B$3:$B$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -720,20 +710,20 @@
     <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Actual (beyond plan) legend" xfId="17" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Actual legend" xfId="15" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Explanatory Text" xfId="12" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="9" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="10" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="11" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Erklärender Text" xfId="12" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
     <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
     <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
     <cellStyle name="Period Value" xfId="13" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
     <cellStyle name="Plan legend" xfId="14" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
     <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Überschrift" xfId="8" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1" xfId="1" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="9" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Überschrift 3" xfId="10" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Überschrift 4" xfId="11" builtinId="19" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
@@ -1128,20 +1118,20 @@
   </sheetPr>
   <dimension ref="B1:AL25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.796875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="22.19921875" style="2" customWidth="1"/>
-    <col min="3" max="6" width="8.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1328125" style="4" customWidth="1"/>
-    <col min="8" max="25" width="4.1328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.625" customWidth="1"/>
+    <col min="2" max="2" width="22.25" style="2" customWidth="1"/>
+    <col min="3" max="6" width="8.375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.125" style="4" customWidth="1"/>
+    <col min="8" max="25" width="4.125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:38" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.6">
+    <row r="1" spans="2:38" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
       <c r="B1" s="9" t="s">
         <v>11</v>
       </c>
@@ -1151,7 +1141,7 @@
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="2:38" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:38" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="10"/>
       <c r="C2" s="16" t="s">
         <v>10</v>
@@ -1189,7 +1179,7 @@
       <c r="Z2" s="19"/>
       <c r="AA2" s="19"/>
     </row>
-    <row r="3" spans="2:38" s="7" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:38" s="7" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" s="38" t="s">
         <v>0</v>
       </c>
@@ -1230,7 +1220,7 @@
       <c r="X3" s="6"/>
       <c r="Y3" s="26"/>
     </row>
-    <row r="4" spans="2:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="39"/>
       <c r="C4" s="37"/>
       <c r="D4" s="37"/>
@@ -1309,7 +1299,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="21" t="s">
         <v>13</v>
       </c>
@@ -1326,7 +1316,7 @@
         <v>4</v>
       </c>
       <c r="G5" s="25">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="H5" s="23"/>
       <c r="I5" s="23"/>
@@ -1347,7 +1337,7 @@
       <c r="X5" s="23"/>
       <c r="Y5" s="24"/>
     </row>
-    <row r="6" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="21" t="s">
         <v>14</v>
       </c>
@@ -1358,13 +1348,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="22">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="F6" s="22">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G6" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="23"/>
       <c r="I6" s="23"/>
@@ -1385,7 +1375,7 @@
       <c r="X6" s="23"/>
       <c r="Y6" s="24"/>
     </row>
-    <row r="7" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="21" t="s">
         <v>15</v>
       </c>
@@ -1396,13 +1386,13 @@
         <v>2</v>
       </c>
       <c r="E7" s="22">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="F7" s="22">
         <v>0</v>
       </c>
       <c r="G7" s="25">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="H7" s="23"/>
       <c r="I7" s="23"/>
@@ -1423,7 +1413,7 @@
       <c r="X7" s="23"/>
       <c r="Y7" s="24"/>
     </row>
-    <row r="8" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="21" t="s">
         <v>16</v>
       </c>
@@ -1462,7 +1452,7 @@
       <c r="Y8" s="24"/>
       <c r="AL8" s="20"/>
     </row>
-    <row r="9" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="21" t="s">
         <v>17</v>
       </c>
@@ -1500,7 +1490,7 @@
       <c r="X9" s="23"/>
       <c r="Y9" s="24"/>
     </row>
-    <row r="10" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="21" t="s">
         <v>18</v>
       </c>
@@ -1538,7 +1528,7 @@
       <c r="X10" s="23"/>
       <c r="Y10" s="24"/>
     </row>
-    <row r="11" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="21" t="s">
         <v>26</v>
       </c>
@@ -1576,7 +1566,7 @@
       <c r="X11" s="23"/>
       <c r="Y11" s="24"/>
     </row>
-    <row r="12" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="21" t="s">
         <v>25</v>
       </c>
@@ -1614,7 +1604,7 @@
       <c r="X12" s="23"/>
       <c r="Y12" s="24"/>
     </row>
-    <row r="13" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="21" t="s">
         <v>19</v>
       </c>
@@ -1652,7 +1642,7 @@
       <c r="X13" s="23"/>
       <c r="Y13" s="24"/>
     </row>
-    <row r="14" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="21" t="s">
         <v>20</v>
       </c>
@@ -1690,7 +1680,7 @@
       <c r="X14" s="23"/>
       <c r="Y14" s="24"/>
     </row>
-    <row r="15" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="21" t="s">
         <v>24</v>
       </c>
@@ -1728,7 +1718,7 @@
       <c r="X15" s="23"/>
       <c r="Y15" s="24"/>
     </row>
-    <row r="16" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="21" t="s">
         <v>27</v>
       </c>
@@ -1766,7 +1756,7 @@
       <c r="X16" s="23"/>
       <c r="Y16" s="24"/>
     </row>
-    <row r="17" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="21" t="s">
         <v>28</v>
       </c>
@@ -1804,7 +1794,7 @@
       <c r="X17" s="23"/>
       <c r="Y17" s="24"/>
     </row>
-    <row r="18" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="21" t="s">
         <v>29</v>
       </c>
@@ -1842,7 +1832,7 @@
       <c r="X18" s="23"/>
       <c r="Y18" s="24"/>
     </row>
-    <row r="19" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="21"/>
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
@@ -1868,7 +1858,7 @@
       <c r="X19" s="23"/>
       <c r="Y19" s="24"/>
     </row>
-    <row r="20" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="21" t="s">
         <v>30</v>
       </c>
@@ -1906,7 +1896,7 @@
       <c r="X20" s="23"/>
       <c r="Y20" s="24"/>
     </row>
-    <row r="21" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="21" t="s">
         <v>31</v>
       </c>
@@ -1944,7 +1934,7 @@
       <c r="X21" s="23"/>
       <c r="Y21" s="24"/>
     </row>
-    <row r="22" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="21" t="s">
         <v>32</v>
       </c>
@@ -1982,7 +1972,7 @@
       <c r="X22" s="23"/>
       <c r="Y22" s="24"/>
     </row>
-    <row r="23" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="21" t="s">
         <v>33</v>
       </c>
@@ -2020,7 +2010,7 @@
       <c r="X23" s="23"/>
       <c r="Y23" s="24"/>
     </row>
-    <row r="24" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="21" t="s">
         <v>23</v>
       </c>
@@ -2058,7 +2048,7 @@
       <c r="X24" s="23"/>
       <c r="Y24" s="24"/>
     </row>
-    <row r="25" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="27" t="s">
         <v>22</v>
       </c>

</xml_diff>